<commit_message>
bf: pretas2 - improve enrollement form.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Burkina Faso/2021/bf_lf_pretas_2_enrolement_2021609.xlsx
+++ b/LF/PreTAS/Burkina Faso/2021/bf_lf_pretas_2_enrolement_2021609.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Burkina Faso\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9730DA8-B666-4F5D-88F0-F23C051FB927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0218828D-E061-43F1-90F1-89D6484EB46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -509,9 +509,6 @@
     <t>${p_sex}='M' and ${p_consent} = '1_oui'</t>
   </si>
   <si>
-    <t>concat(${p_recorder_id},'-', ${Numero_famille},'-',${Numero_Enquete})</t>
-  </si>
-  <si>
     <t xml:space="preserve">string-length(.)=10 </t>
   </si>
   <si>
@@ -558,13 +555,16 @@
     </r>
   </si>
   <si>
-    <t>(BF - Juin 2021) Pré TAS FL - 2. Formulaire Enrôlement V2.1</t>
-  </si>
-  <si>
-    <t>bf_lf_pretas_2_enrolement_202106_v2_1</t>
-  </si>
-  <si>
-    <t>Le code doit être trois 3 chiffres</t>
+    <t>concat(${p_cluster_id}, '-',${p_recorder_id},'-', ${Numero_famille},'-',${Numero_Enquete})</t>
+  </si>
+  <si>
+    <t>Le code doit être 3 chiffres</t>
+  </si>
+  <si>
+    <t>(BF - Juin 2021) Pré TAS FL - 2. Formulaire Enrôlement V2.2</t>
+  </si>
+  <si>
+    <t>bf_lf_pretas_2_enrolement_202106_v2_2</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1225,7 +1225,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>10</v>
@@ -1262,7 +1262,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1360,7 +1360,7 @@
         <v>111</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>109</v>
@@ -1386,10 +1386,10 @@
         <v>111</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>140</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="12" spans="1:14" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A12" s="7" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>114</v>
@@ -1409,13 +1409,13 @@
         <v>62</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>128</v>
@@ -1455,7 +1455,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" s="10" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A14" s="7" t="s">
         <v>74</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>128</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -1580,10 +1580,10 @@
         <v>56</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>129</v>
@@ -1665,7 +1665,7 @@
         <v>127</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>131</v>
@@ -1712,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -2049,7 +2049,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2075,10 +2075,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2">
         <v>20210605</v>

</xml_diff>